<commit_message>
cost per 20 years is added
</commit_message>
<xml_diff>
--- a/Project 1/Transformer Calculator Gokhan.xlsx
+++ b/Project 1/Transformer Calculator Gokhan.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
   <si>
     <t>A</t>
   </si>
@@ -276,9 +276,6 @@
       </rPr>
       <t>$</t>
     </r>
-  </si>
-  <si>
-    <t>Total Cost</t>
   </si>
   <si>
     <t>Core Material Cost</t>
@@ -413,6 +410,29 @@
         <scheme val="minor"/>
       </rPr>
       <t>core</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Production Cost</t>
+  </si>
+  <si>
+    <t>Total Losses for 20 Years</t>
+  </si>
+  <si>
+    <t>Electricity Price</t>
+  </si>
+  <si>
+    <r>
+      <t>₺/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial Tur"/>
+        <charset val="162"/>
+      </rPr>
+      <t>kWh</t>
     </r>
   </si>
 </sst>
@@ -743,6 +763,15 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,15 +809,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1205,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1229,67 +1249,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="A1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="16" t="s">
@@ -1302,24 +1322,24 @@
         <v>6</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
+      <c r="G4" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="30"/>
+      <c r="L4" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="33"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1332,7 +1352,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1340,13 +1360,13 @@
       </c>
       <c r="I5" s="2">
         <f>ROUND(vin*C4/C5,0)</f>
-        <v>1490</v>
+        <v>1449</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="22" t="s">
         <v>43</v>
       </c>
       <c r="M5" s="3" t="s">
@@ -1354,7 +1374,7 @@
       </c>
       <c r="N5" s="11">
         <f>0.000000017*I17/(I10/1000000)*(1+0.004041*(C11-20))</f>
-        <v>6.7654699040326722</v>
+        <v>6.6175386789036708</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>44</v>
@@ -1362,20 +1382,20 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <v>1080</v>
+        <v>1050</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="22" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -1389,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="22" t="s">
         <v>45</v>
       </c>
       <c r="M6" s="3" t="s">
@@ -1397,7 +1417,7 @@
       </c>
       <c r="N6" s="11">
         <f>0.000000017*I19/(I11/1000000)*(1+0.004041*(C11-20))</f>
-        <v>3.626020803361901</v>
+        <v>3.5457837054595758</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>44</v>
@@ -1405,7 +1425,7 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1418,7 +1438,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1432,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="22" t="s">
         <v>46</v>
       </c>
       <c r="M7" s="3" t="s">
@@ -1440,15 +1460,15 @@
       </c>
       <c r="N7" s="11">
         <f>I7^2*N5/1000</f>
-        <v>1.4796112800862209</v>
+        <v>1.4472586552896227</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -1461,7 +1481,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1469,13 +1489,13 @@
       </c>
       <c r="I8" s="14">
         <f>C4*1000/4.44/I5/C9/C8*10000</f>
-        <v>695.32619868190329</v>
+        <v>715.00071500071499</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="6"/>
-      <c r="L8" s="35" t="s">
+      <c r="L8" s="22" t="s">
         <v>47</v>
       </c>
       <c r="M8" s="3" t="s">
@@ -1483,15 +1503,15 @@
       </c>
       <c r="N8" s="11">
         <f>I6^2*N6/1000</f>
-        <v>1.4504083213447605</v>
+        <v>1.4183134821838304</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -1504,7 +1524,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -1512,29 +1532,29 @@
       </c>
       <c r="I9" s="11">
         <f>SQRT(I8)</f>
-        <v>26.369038637802163</v>
+        <v>26.73949728399386</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K9" s="6"/>
-      <c r="L9" s="35" t="s">
-        <v>81</v>
+      <c r="L9" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N9" s="11">
         <f>N8+N7</f>
-        <v>2.9300196014309812</v>
+        <v>2.8655721374734533</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -1547,8 +1567,8 @@
         <v>23</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="35" t="s">
-        <v>74</v>
+      <c r="G10" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>1</v>
@@ -1561,7 +1581,7 @@
         <v>24</v>
       </c>
       <c r="K10" s="6"/>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="22" t="s">
         <v>33</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1569,16 +1589,16 @@
       </c>
       <c r="N10" s="11">
         <f>C15*I23/1000</f>
-        <v>2.6974194722174034</v>
+        <v>2.7774102565184737</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>71</v>
+      <c r="A11" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>1</v>
@@ -1587,11 +1607,11 @@
         <v>50</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="35" t="s">
-        <v>75</v>
+      <c r="G11" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>1</v>
@@ -1604,7 +1624,7 @@
         <v>24</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="L11" s="35" t="s">
+      <c r="L11" s="22" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="3" t="s">
@@ -1612,15 +1632,15 @@
       </c>
       <c r="N11" s="11">
         <f>(N8+N7+N10)</f>
-        <v>5.6274390736483841</v>
+        <v>5.642982393991927</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -1631,7 +1651,7 @@
       </c>
       <c r="D12" s="16"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="22" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="3" t="s">
@@ -1639,13 +1659,13 @@
       </c>
       <c r="I12" s="14">
         <f>(I5*I10+vin*I11)/fs/100</f>
-        <v>484.83223240987223</v>
+        <v>471.4285714285715</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K12" s="6"/>
-      <c r="L12" s="35" t="s">
+      <c r="L12" s="22" t="s">
         <v>49</v>
       </c>
       <c r="M12" s="3" t="s">
@@ -1653,15 +1673,15 @@
       </c>
       <c r="N12" s="13">
         <f>100*(VOUT*1000*pbudget)/(VOUT*1000*pbudget+N11*1000)</f>
-        <v>98.887038432099672</v>
+        <v>98.883998672882811</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1674,15 +1694,15 @@
         <v>30</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="35" t="s">
-        <v>82</v>
+      <c r="G13" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="11">
         <f>SQRT(I12)</f>
-        <v>22.018906249173057</v>
+        <v>21.712405933672379</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>19</v>
@@ -1695,7 +1715,7 @@
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="16" t="s">
@@ -1708,30 +1728,30 @@
         <v>30</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="35" t="s">
-        <v>83</v>
+      <c r="G14" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I14" s="11">
         <f>I13+2*I9</f>
-        <v>74.756983524777382</v>
+        <v>75.191400501660098</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
+      <c r="L14" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1749,7 +1769,7 @@
       <c r="I15" s="19"/>
       <c r="J15" s="6"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="35" t="s">
+      <c r="L15" s="22" t="s">
         <v>51</v>
       </c>
       <c r="M15" s="3" t="s">
@@ -1757,15 +1777,15 @@
       </c>
       <c r="N15" s="14">
         <f>0.04*(I9+I13)/(vrdson*PI()*0.0000004*I8/10000)</f>
-        <v>26688.28207197761</v>
+        <v>25988.211940152643</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1776,14 +1796,14 @@
       </c>
       <c r="D16" s="16"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="G16" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="35" t="s">
+      <c r="L16" s="22" t="s">
         <v>53</v>
       </c>
       <c r="M16" s="3" t="s">
@@ -1791,7 +1811,7 @@
       </c>
       <c r="N16" s="11">
         <f>I5^2/N15</f>
-        <v>83.186321023303321</v>
+        <v>80.790513977456342</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>54</v>
@@ -1799,7 +1819,7 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -1810,7 +1830,7 @@
       </c>
       <c r="D17" s="16"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="22" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="3" t="s">
@@ -1818,14 +1838,14 @@
       </c>
       <c r="I17" s="14">
         <f>PI()*(I9+I13/2)*I5/100</f>
-        <v>1749.6771273325048</v>
+        <v>1711.4193441041427</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K17" s="6"/>
-      <c r="L17" s="35" t="s">
-        <v>77</v>
+      <c r="L17" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>1</v>
@@ -1840,8 +1860,8 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
-        <v>60</v>
+      <c r="A18" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>1</v>
@@ -1850,10 +1870,10 @@
         <v>10</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="22" t="s">
         <v>37</v>
       </c>
       <c r="H18" s="3" t="s">
@@ -1861,14 +1881,14 @@
       </c>
       <c r="I18" s="14">
         <f>C14*I17*I10/1000000</f>
-        <v>77.280425223795945</v>
+        <v>75.590640457325847</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="K18" s="6"/>
-      <c r="L18" s="35" t="s">
-        <v>78</v>
+      <c r="L18" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>1</v>
@@ -1878,13 +1898,13 @@
         <v>148.5163900758607</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
-        <v>58</v>
+      <c r="A19" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>1</v>
@@ -1893,10 +1913,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="5"/>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="22" t="s">
         <v>39</v>
       </c>
       <c r="H19" s="3" t="s">
@@ -1904,29 +1924,29 @@
       </c>
       <c r="I19" s="14">
         <f>PI()*(I9+I13/2)*vin/100</f>
-        <v>1268.2223473282586</v>
+        <v>1240.1589450030021</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K19" s="6"/>
-      <c r="L19" s="35" t="s">
-        <v>79</v>
+      <c r="L19" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N19" s="11">
         <f>N18*vin^2/I5^2</f>
-        <v>78.027799371417473</v>
+        <v>77.985922115028728</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1939,7 +1959,7 @@
         <v>56</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="35" t="s">
+      <c r="G20" s="22" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="3" t="s">
@@ -1947,7 +1967,7 @@
       </c>
       <c r="I20" s="14">
         <f>C14*I19*I11/1000000</f>
-        <v>75.755148213741322</v>
+        <v>74.078827648179342</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>32</v>
@@ -1960,8 +1980,20 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="22" t="s">
         <v>41</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -1969,23 +2001,23 @@
       </c>
       <c r="I21" s="14">
         <f>I20+I18</f>
-        <v>153.03557343753727</v>
+        <v>149.66946810550519</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="22"/>
+      <c r="L21" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="25"/>
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F22" s="5"/>
-      <c r="G22" s="35" t="s">
+      <c r="G22" s="22" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="3" t="s">
@@ -1993,30 +2025,30 @@
       </c>
       <c r="I22" s="13">
         <f>((I13+2*I9)^2-(I13)^2)*I9/1000000</f>
-        <v>0.13458162312115968</v>
+        <v>0.13857258177510723</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K22" s="7"/>
-      <c r="L22" s="35" t="s">
-        <v>61</v>
+      <c r="L22" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N22" s="12">
         <f>C19*I23*dmax</f>
-        <v>12045.728177459396</v>
+        <v>12402.938931780973</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F23" s="5"/>
-      <c r="G23" s="35" t="s">
+      <c r="G23" s="22" t="s">
         <v>31</v>
       </c>
       <c r="H23" s="3" t="s">
@@ -2024,30 +2056,30 @@
       </c>
       <c r="I23" s="14">
         <f>I22*C13</f>
-        <v>1029.5494168768714</v>
+        <v>1060.0802505795702</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="6"/>
-      <c r="L23" s="35" t="s">
-        <v>60</v>
+      <c r="L23" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N23" s="12">
         <f>C18*I21*dmax</f>
-        <v>5968.387364063954</v>
+        <v>5837.1092561147025</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F24" s="5"/>
-      <c r="G24" s="35" t="s">
+      <c r="G24" s="22" t="s">
         <v>42</v>
       </c>
       <c r="H24" s="3" t="s">
@@ -2055,24 +2087,24 @@
       </c>
       <c r="I24" s="14">
         <f>I21+I23</f>
-        <v>1182.5849903144087</v>
+        <v>1209.7497186850755</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>32</v>
       </c>
       <c r="K24" s="7"/>
-      <c r="L24" s="35" t="s">
-        <v>57</v>
+      <c r="L24" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N24" s="12">
         <f>N23+N22</f>
-        <v>18014.115541523352</v>
+        <v>18240.048187895674</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
@@ -2082,20 +2114,29 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="L25" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" s="12">
+        <f>N11*_ta1*24*365*20</f>
+        <v>395460.20617095428</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G30" s="33" t="s">
-        <v>73</v>
+      <c r="G30" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" deleteRows="0" sort="0"/>
   <protectedRanges>
-    <protectedRange sqref="C4:C20" name="Aralık1"/>
+    <protectedRange sqref="C4:C21" name="Aralık1"/>
   </protectedRanges>
   <mergeCells count="8">
     <mergeCell ref="L21:O21"/>

</xml_diff>